<commit_message>
added shift pulse and onbstacledetection switch
</commit_message>
<xml_diff>
--- a/ProjectDocumention/PlanDeConvergenceIntegration.xlsx
+++ b/ProjectDocumention/PlanDeConvergenceIntegration.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9990" yWindow="0" windowWidth="19200" windowHeight="11265"/>
+    <workbookView xWindow="16650" yWindow="0" windowWidth="19200" windowHeight="11265"/>
   </bookViews>
   <sheets>
     <sheet name="Liste de tâches" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="66">
   <si>
     <r>
       <rPr>
@@ -184,9 +184,6 @@
     <t>Debug AStarSearch ne trouve pas le chemin entre (370,250) et (55,55)</t>
   </si>
   <si>
-    <t>alors que le trajet inverse est ok</t>
-  </si>
-  <si>
     <t xml:space="preserve">Comprendre / debug pourquoi les particules vont toujours plus loin que le robot </t>
   </si>
   <si>
@@ -255,6 +252,69 @@
     <t>java: créer un retcode specifique pour octave qui fera la simu
 fait une v0 - et v1 reste a valider en reel
 reste a testes java pour ne pas envoyer pingFB vers le robot si simu</t>
+  </si>
+  <si>
+    <t>Debuguer restart apres detection  obstacle</t>
+  </si>
+  <si>
+    <t>Debuger timeout Ping FB apres motors status 0x06</t>
+  </si>
+  <si>
+    <t>alors que le trajet inverse est ok
+reecriture complete du astar realisee</t>
+  </si>
+  <si>
+    <t>Debuger test echo consistancy en reel</t>
+  </si>
+  <si>
+    <t>Debuger theoritical heading à 0</t>
+  </si>
+  <si>
+    <t>correction a verifier</t>
+  </si>
+  <si>
+    <t>Verifier coherence de la carto</t>
+  </si>
+  <si>
+    <t>cf 2016/09/28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gerer dans octave les differents timeout </t>
+  </si>
+  <si>
+    <t>Ajouter timer apres ack java vers robot avant envoi trame suivante</t>
+  </si>
+  <si>
+    <t>pour laisser le temps a arduino de traiter</t>
+  </si>
+  <si>
+    <t>Debuguer envoi successif de echo de java vers robot</t>
+  </si>
+  <si>
+    <t>provisoirement mis en commentaire 
+en effet si obstacle on envoit end move mais le mouvement  reprend ensuite avec un nouveau endmove alors qu'entre temps octave a valider la position</t>
+  </si>
+  <si>
+    <t>valeurs toujours tres faibles ! Non significatives
+re-ecriture du code octave</t>
+  </si>
+  <si>
+    <t>a tester</t>
+  </si>
+  <si>
+    <t>Remonter les data encodeurs en fin de move</t>
+  </si>
+  <si>
+    <t>pour analyse de comportement (anomalies et tunning)</t>
+  </si>
+  <si>
+    <t>Analyser les data encodeurs</t>
+  </si>
+  <si>
+    <t>Ajouter un timer mini a sendUDP entre 2 trames</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corriger NO robot à 0 au demarrage </t>
   </si>
 </sst>
 </file>
@@ -698,7 +758,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Title" descr="Liste de tâches" title="Titre de modèle"/>
+        <xdr:cNvPr id="2" name="Title" descr="Liste de tâches" title="Titre de modèle">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -773,7 +839,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="To Do Year" descr="Contient l’année de la liste de tâches (2014, par exemple)" title="Année de la liste de tâches"/>
+        <xdr:cNvPr id="3" name="To Do Year" descr="Contient l’année de la liste de tâches (2014, par exemple)" title="Année de la liste de tâches">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -824,8 +896,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Liste_de_tâches" displayName="Liste_de_tâches" ref="B4:I21" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B4:I21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Liste_de_tâches" displayName="Liste_de_tâches" ref="B4:I33" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B4:I33">
     <filterColumn colId="2">
       <filters>
         <filter val="En cours de réalisation"/>
@@ -1095,10 +1167,10 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:I21"/>
+  <dimension ref="B1:I33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1160,7 +1232,7 @@
       </c>
       <c r="F5" s="8">
         <f ca="1">TODAY()-1</f>
-        <v>42583</v>
+        <v>42669</v>
       </c>
       <c r="G5" s="4">
         <v>1</v>
@@ -1173,13 +1245,13 @@
     </row>
     <row r="6" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -1191,27 +1263,27 @@
         <v>2</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="2">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="3"/>
     </row>
@@ -1242,13 +1314,13 @@
     </row>
     <row r="9" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="9">
         <v>42579</v>
@@ -1262,7 +1334,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1283,7 +1355,7 @@
         <v>2</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1321,7 +1393,7 @@
         <v>15</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -1342,28 +1414,30 @@
         <v>15</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="12"/>
+      <c r="G13" s="7">
+        <v>1</v>
+      </c>
       <c r="H13" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -1375,12 +1449,12 @@
         <v>2</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>15</v>
@@ -1402,43 +1476,43 @@
         <v>1</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E16" s="9">
         <v>42579</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H16" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -1448,12 +1522,12 @@
         <v>2</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>15</v>
@@ -1469,12 +1543,12 @@
         <v>2</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>10</v>
@@ -1490,18 +1564,18 @@
         <v>2</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -1513,7 +1587,7 @@
         <v>2</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1529,9 +1603,259 @@
       </c>
       <c r="I21" s="5"/>
     </row>
+    <row r="22" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="H24" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="H25" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="7">
+        <v>1</v>
+      </c>
+      <c r="H28" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>1</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="H30" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="7">
+        <v>1</v>
+      </c>
+      <c r="H31" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>1</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="7">
+        <v>1</v>
+      </c>
+      <c r="H33" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>1</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G5:G21">
+  <conditionalFormatting sqref="G5:G33">
     <cfRule type="dataBar" priority="59">
       <dataBar>
         <cfvo type="min"/>
@@ -1546,17 +1870,17 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" sqref="G5:G21">
+    <dataValidation type="list" allowBlank="1" sqref="G5:G33">
       <formula1>"0%,25%,50%,75%,100%"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Whoops" sqref="C5:C21">
+    <dataValidation type="list" allowBlank="1" errorTitle="Whoops" sqref="C5:C33">
       <formula1>"Basse, Normale, Élevée"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly you need to select a choice from the drop down list. But you can still use what you entered by clicking Yes." sqref="D5:D21">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly, your Due Date needs to be greater than or equal to the Start Date." sqref="F5:F33">
+      <formula1>F5&gt;=E5</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly you need to select a choice from the drop down list. But you can still use what you entered by clicking Yes." sqref="D5:D33 B22">
       <formula1>"Non commencée,En cours de réalisation, Différé, Terminée"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly, your Due Date needs to be greater than or equal to the Start Date." sqref="F5:F21">
-      <formula1>F5&gt;=E5</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
@@ -1582,7 +1906,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G5:G21</xm:sqref>
+          <xm:sqref>G5:G33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="60" id="{61976558-4184-4BD1-B78A-DCBE6FDA3BC9}">
@@ -1601,7 +1925,7 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>H5:H21</xm:sqref>
+          <xm:sqref>H5:H33</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1616,6 +1940,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated for BNO055 support
</commit_message>
<xml_diff>
--- a/ProjectDocumention/PlanDeConvergenceIntegration.xlsx
+++ b/ProjectDocumention/PlanDeConvergenceIntegration.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="163">
   <si>
     <r>
       <rPr>
@@ -514,9 +514,6 @@
     <t>Ne pas prendre en compte les resultats de echoconsistancy au dessous d'un certain seuil</t>
   </si>
   <si>
-    <t>seuil a determiner - pour conserver les memes prob que le mseure precedente</t>
-  </si>
-  <si>
     <t>Tuner le filtre a particules / poids des mesures</t>
   </si>
   <si>
@@ -543,31 +540,79 @@
     <t>Utiliser accelerometre pour detecter les chocs</t>
   </si>
   <si>
-    <t>Affiner carto en tenant compte des arronids</t>
-  </si>
-  <si>
     <t>Debuger trajet en marche arriere</t>
   </si>
   <si>
     <t>ok with simultaor to be validated with real robot</t>
   </si>
   <si>
-    <t>le magnetometre ne semble pas fonctionner !</t>
-  </si>
-  <si>
-    <t>semble une bonne piste mais qui necessite de revoir largement le sous systeme</t>
-  </si>
-  <si>
     <t>Ajouter dispo surveillance alim moteurs</t>
   </si>
   <si>
-    <t>corriger Jeu roue gauche sur axe</t>
-  </si>
-  <si>
-    <t>Considerer le centre du robot comme reference de la position</t>
-  </si>
-  <si>
-    <t>pour simplifier les calcules - compenser entre contre partie les echos</t>
+    <t>juste serrage des vis</t>
+  </si>
+  <si>
+    <t>juste realise le calcul du decalage lie au centre de rotation sur base gyro</t>
+  </si>
+  <si>
+    <t>Affiner carto en tenant compte des arrondis</t>
+  </si>
+  <si>
+    <t>Corriger Jeu roue gauche sur axe</t>
+  </si>
+  <si>
+    <t>Debuger decalage entre theo et particles</t>
+  </si>
+  <si>
+    <t>Reparer panne alimentation 5 et 9v</t>
+  </si>
+  <si>
+    <t>remplacement des 2 modules - 5v a l identique 9 v par regulateur integre</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> remplace par une ponderation des mesures en entree de determine particles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reste a valider en reel </t>
+  </si>
+  <si>
+    <t>Ecrire une fonction de test echo consistency basee sur les echos en BD et non la carto</t>
+  </si>
+  <si>
+    <t>developpement fait - voir si cela donne de meilleurs resultats que sur base carto</t>
+  </si>
+  <si>
+    <t>Tunner les dimensions physiques du robot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diametre des roues ajustes </t>
+  </si>
+  <si>
+    <t>Developper la fonction de calcul de la position relative dans le sous-système</t>
+  </si>
+  <si>
+    <t>necessite que le robot communique regulierement le deplacement</t>
+  </si>
+  <si>
+    <t>gyroscope: semble une bonne piste mais qui necessite de revoir largement le sous système</t>
+  </si>
+  <si>
+    <t>plus precis que le developpement maison (BNO055 en mode IMU)</t>
+  </si>
+  <si>
+    <t>Utiliser BNO055 pour valider la fonction gyroscope</t>
+  </si>
+  <si>
+    <t>le magnetometre ne semble pas fonctionner et le BNO055 une meilleure solution</t>
+  </si>
+  <si>
+    <t>Utiliser la fonction magnetometre du BNO055</t>
+  </si>
+  <si>
+    <t>POC utilisation de l'accelerometre BNO055 pour detecter les chocs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">necessite de developper une fonction de switch des modes </t>
   </si>
 </sst>
 </file>
@@ -1167,8 +1212,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Liste_de_tâches" displayName="Liste_de_tâches" ref="B4:I75" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B4:I75"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Liste_de_tâches" displayName="Liste_de_tâches" ref="B4:I82" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B4:I82"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Tâche" dataDxfId="7"/>
     <tableColumn id="3" name="Priorité " dataDxfId="6"/>
@@ -1431,10 +1476,10 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:N75"/>
+  <dimension ref="B1:N82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L73" sqref="L73"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I83" sqref="I83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1496,7 +1541,7 @@
       </c>
       <c r="F5" s="8">
         <f ca="1">TODAY()-1</f>
-        <v>42739</v>
+        <v>42741</v>
       </c>
       <c r="G5" s="4">
         <v>1</v>
@@ -2524,7 +2569,7 @@
         <v>2</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2669,7 +2714,7 @@
         <v>12</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
@@ -2690,7 +2735,7 @@
         <v>15</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E60" s="9"/>
       <c r="F60" s="9"/>
@@ -2700,7 +2745,7 @@
         <v>2</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2715,13 +2760,15 @@
       </c>
       <c r="E61" s="9"/>
       <c r="F61" s="9"/>
-      <c r="G61" s="12"/>
+      <c r="G61" s="7">
+        <v>0.25</v>
+      </c>
       <c r="H61" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
     </row>
     <row r="62" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2743,7 +2790,9 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I62" s="5"/>
+      <c r="I62" s="5" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="63" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="s">
@@ -2757,7 +2806,9 @@
       </c>
       <c r="E63" s="9"/>
       <c r="F63" s="9"/>
-      <c r="G63" s="12"/>
+      <c r="G63" s="7">
+        <v>0.25</v>
+      </c>
       <c r="H63" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
@@ -2793,30 +2844,36 @@
         <v>12</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="E65" s="9"/>
       <c r="F65" s="9"/>
-      <c r="G65" s="12"/>
+      <c r="G65" s="7">
+        <v>1</v>
+      </c>
       <c r="H65" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
     </row>
     <row r="66" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D66" s="5"/>
+      <c r="D66" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="E66" s="9"/>
       <c r="F66" s="9"/>
-      <c r="G66" s="12"/>
+      <c r="G66" s="7">
+        <v>0.5</v>
+      </c>
       <c r="H66" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
@@ -2825,7 +2882,7 @@
     </row>
     <row r="67" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>12</v>
@@ -2843,12 +2900,12 @@
         <v>2</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>10</v>
@@ -2866,29 +2923,35 @@
         <v>2</v>
       </c>
       <c r="I68" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D69" s="5"/>
+      <c r="D69" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="E69" s="9"/>
       <c r="F69" s="9"/>
-      <c r="G69" s="12"/>
+      <c r="G69" s="7">
+        <v>0.25</v>
+      </c>
       <c r="H69" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I69" s="5"/>
+      <c r="I69" s="5" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="70" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>10</v>
@@ -2905,7 +2968,7 @@
     </row>
     <row r="71" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="5" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>12</v>
@@ -2926,7 +2989,7 @@
     </row>
     <row r="72" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>12</v>
@@ -2944,12 +3007,12 @@
         <v>2</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>10</v>
@@ -2966,7 +3029,7 @@
     </row>
     <row r="74" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>10</v>
@@ -2983,30 +3046,181 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>1</v>
       </c>
-      <c r="I74" s="5"/>
+      <c r="I74" s="5" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="75" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D75" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
-      <c r="G75" s="12"/>
+      <c r="G75" s="7">
+        <v>0.5</v>
+      </c>
       <c r="H75" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I75" s="5" t="s">
+      <c r="I75" s="5"/>
+    </row>
+    <row r="76" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="7">
+        <v>1</v>
+      </c>
+      <c r="H76" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>1</v>
+      </c>
+      <c r="I76" s="5" t="s">
         <v>147</v>
       </c>
+    </row>
+    <row r="77" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="H77" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I77" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="H78" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I78" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" s="5"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I79" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="7">
+        <v>1</v>
+      </c>
+      <c r="H80" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I80" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81" s="5"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="12"/>
+      <c r="H81" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I81" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D82" s="5"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="12"/>
+      <c r="H82" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I82" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G5:G75">
+  <conditionalFormatting sqref="G5:G82">
     <cfRule type="dataBar" priority="59">
       <dataBar>
         <cfvo type="min"/>
@@ -3021,16 +3235,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" sqref="G5:G75">
+    <dataValidation type="list" allowBlank="1" sqref="G5:G82">
       <formula1>"0%,25%,50%,75%,100%"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Whoops" sqref="C5:C75">
+    <dataValidation type="list" allowBlank="1" errorTitle="Whoops" sqref="C5:C82">
       <formula1>"Basse, Normale, Élevée"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly, your Due Date needs to be greater than or equal to the Start Date." sqref="F5:F75">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly, your Due Date needs to be greater than or equal to the Start Date." sqref="F5:F82">
       <formula1>F5&gt;=E5</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly you need to select a choice from the drop down list. But you can still use what you entered by clicking Yes." sqref="D5:D75 B22">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly you need to select a choice from the drop down list. But you can still use what you entered by clicking Yes." sqref="D5:D82 B22">
       <formula1>"Non commencée,En cours de réalisation, Différé, Terminée"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3057,7 +3271,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G5:G75</xm:sqref>
+          <xm:sqref>G5:G82</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="60" id="{61976558-4184-4BD1-B78A-DCBE6FDA3BC9}">
@@ -3076,7 +3290,7 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>H5:H75</xm:sqref>
+          <xm:sqref>H5:H82</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3092,7 +3306,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
+      <selection pane="bottomRight" activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
echo scan added before moves and rotations
</commit_message>
<xml_diff>
--- a/ProjectDocumention/PlanDeConvergenceIntegration.xlsx
+++ b/ProjectDocumention/PlanDeConvergenceIntegration.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="28860" yWindow="0" windowWidth="19200" windowHeight="11265"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="174">
   <si>
     <r>
       <rPr>
@@ -161,9 +161,6 @@
   </si>
   <si>
     <t>Debug  "DetermineRobotLocationWithParticlesGaussian()"</t>
-  </si>
-  <si>
-    <t>alors que le robot est pose sur socle</t>
   </si>
   <si>
     <r>
@@ -196,9 +193,6 @@
     <t xml:space="preserve"> Modifier traitements particules quand le robot interromp son deplacement (ex motor diag=0x04 et obstacle)</t>
   </si>
   <si>
-    <t>se declenche tres souvent</t>
-  </si>
-  <si>
     <t>refaire le move particules avec distance inferieure
 utiliser le retCode actionEnd</t>
   </si>
@@ -212,14 +206,7 @@
     <t>Ne pas recalculer la trajectoire si on est proche de next step</t>
   </si>
   <si>
-    <t>en grande partie du aux ko lors des deplacements (corrige)
-reste à verifier que le pb a complement disparu</t>
-  </si>
-  <si>
     <t>Fiabiliser robot pbSynchro motor</t>
-  </si>
-  <si>
-    <t>d  abord faire le simulateur fonction pingFB</t>
   </si>
   <si>
     <t>Différé</t>
@@ -267,9 +254,6 @@
     <t>Verifier coherence de la carto</t>
   </si>
   <si>
-    <t>cf 2016/09/28</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gerer dans octave les differents timeout </t>
   </si>
   <si>
@@ -280,9 +264,6 @@
   </si>
   <si>
     <t>Debuguer envoi successif de echo de java vers robot</t>
-  </si>
-  <si>
-    <t>a tester</t>
   </si>
   <si>
     <t>Remonter les data encodeurs en fin de move</t>
@@ -323,9 +304,6 @@
   </si>
   <si>
     <t xml:space="preserve">modifs au fil de l'eau </t>
-  </si>
-  <si>
-    <t>Re-écrire le code Octave test</t>
   </si>
   <si>
     <t>valeurs toujours tres faibles ! Non significatives
@@ -372,12 +350,6 @@
     <t>Basculer mouvement du robot en angle distance VS (X,Y)</t>
   </si>
   <si>
-    <t>Reduire voltage alimentation moteur a 11v</t>
-  </si>
-  <si>
-    <t>pas retenue</t>
-  </si>
-  <si>
     <t>Externaliser les parametres PWM et encodeurs</t>
   </si>
   <si>
@@ -399,9 +371,6 @@
     <t xml:space="preserve">Etudier la possibilite de recalibrer facilement la boussole </t>
   </si>
   <si>
-    <t>pouvoir demonter facilement</t>
-  </si>
-  <si>
     <t>Revoir architecture capteur si POC gyroscope Ok</t>
   </si>
   <si>
@@ -412,9 +381,6 @@
   </si>
   <si>
     <t>Definir un plan de validation des datas gyroscope</t>
-  </si>
-  <si>
-    <t>Necessite externalisation de parametres ODR et range</t>
   </si>
   <si>
     <t>ODR</t>
@@ -534,15 +500,9 @@
     <t>sur la base des echo en BD</t>
   </si>
   <si>
-    <t>Utiliser accelerometre pour detecter les chocs</t>
-  </si>
-  <si>
     <t>Debuger trajet en marche arriere</t>
   </si>
   <si>
-    <t>ok with simultaor to be validated with real robot</t>
-  </si>
-  <si>
     <t>juste serrage des vis</t>
   </si>
   <si>
@@ -603,22 +563,92 @@
     <t>POC utilisation de l'accelerometre BNO055 pour detecter les chocs</t>
   </si>
   <si>
+    <t>necessite que le robot communique regulierement le deplacement / notamment utile quand le robot touche</t>
+  </si>
+  <si>
+    <t>Developper une fonction retrait si blocage des roues</t>
+  </si>
+  <si>
+    <t>Ajouter dispositif surveillance alim moteurs</t>
+  </si>
+  <si>
+    <t>Ajouter un calcul position base sur gyro dans l arduino Mega</t>
+  </si>
+  <si>
+    <t>Ajouter affichage java du statut BNO</t>
+  </si>
+  <si>
+    <t>alors que le robot est pose sur socle
+le pb ne s est pas reproduit</t>
+  </si>
+  <si>
+    <t>en grande partie du aux ko lors des deplacements (corrige)
+reste à verifier que le pb a complement disparu
+clos apres prise en compte du decalage entre centre rotation roue et centre robot</t>
+  </si>
+  <si>
+    <t>se declenche tres souvent
+qq modifs du  code</t>
+  </si>
+  <si>
+    <t>corrige</t>
+  </si>
+  <si>
+    <t>pas retenu</t>
+  </si>
+  <si>
+    <t>Re-écrire le code Octave test trajectory</t>
+  </si>
+  <si>
+    <t>pas pertinent apres usage IMU</t>
+  </si>
+  <si>
+    <t>(reel, test patricules) a valider</t>
+  </si>
+  <si>
     <t xml:space="preserve">necessite de developper une fonction de switch des modes </t>
   </si>
   <si>
-    <t>necessite que le robot communique regulierement le deplacement / notamment utile quand le robot touche</t>
-  </si>
-  <si>
-    <t>Developper une fonction retrait si blocage des roues</t>
-  </si>
-  <si>
-    <t>Ajouter dispositif surveillance alim moteurs</t>
-  </si>
-  <si>
-    <t>Ajouter un calcul position base sur gyro dans l arduino Mega</t>
-  </si>
-  <si>
-    <t>Ajouter affichage java du statut BNO</t>
+    <t>Necessite externalisation de parametres ODR et range fait mais plus necessaire avec IMU</t>
+  </si>
+  <si>
+    <t>pouvoir demonter facilement - plus necessaire avec IMU</t>
+  </si>
+  <si>
+    <t>Reduire voltage alimentation moteur a 10v</t>
+  </si>
+  <si>
+    <t>pour gagner en performance voire en dynamique</t>
+  </si>
+  <si>
+    <t>Revoir la façon de determiner le path (type Voronoi graph ou potentiel field ou probabilistic road map planner ?)</t>
+  </si>
+  <si>
+    <t>Rechercer des bibliothques Octave pour accroitre performance de l analyse  echo (cf biblio python)</t>
+  </si>
+  <si>
+    <t>dans Octave traduire les coordonnees du robot sous forme de matrice (x,y,theta)</t>
+  </si>
+  <si>
+    <t>Ameliorer la detection d obstacle pour eviter les contacts</t>
+  </si>
+  <si>
+    <t>En cas de code retour move negatif augmenter le sigma du move particules</t>
+  </si>
+  <si>
+    <t>Prendre en compte dans Octave l'impossibilite de localisation</t>
+  </si>
+  <si>
+    <t>Etendre apprentissage echo au salon &amp; etendre zonexy</t>
+  </si>
+  <si>
+    <t>Tester echolocalisation avec ML rotation virtuelele</t>
+  </si>
+  <si>
+    <t>Avant  move verifier faisabilite avec echo</t>
+  </si>
+  <si>
+    <t>Avant rotation verifier faisabilite avec echo</t>
   </si>
 </sst>
 </file>
@@ -1218,8 +1248,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Liste_de_tâches" displayName="Liste_de_tâches" ref="B4:I84" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B4:I84"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Liste_de_tâches" displayName="Liste_de_tâches" ref="B4:I92" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B4:I92"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Tâche" dataDxfId="7"/>
     <tableColumn id="3" name="Priorité " dataDxfId="6"/>
@@ -1482,10 +1512,10 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:N84"/>
+  <dimension ref="B1:N92"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1547,7 +1577,7 @@
       </c>
       <c r="F5" s="8">
         <f ca="1">TODAY()-1</f>
-        <v>42757</v>
+        <v>42844</v>
       </c>
       <c r="G5" s="4">
         <v>1</v>
@@ -1560,7 +1590,7 @@
     </row>
     <row r="6" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>12</v>
@@ -1581,7 +1611,7 @@
     </row>
     <row r="7" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>10</v>
@@ -1599,7 +1629,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1629,13 +1659,13 @@
     </row>
     <row r="9" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E9" s="9">
         <v>42579</v>
@@ -1649,7 +1679,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1669,9 +1699,7 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
@@ -1702,13 +1730,13 @@
     </row>
     <row r="12" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -1717,13 +1745,13 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I12" s="5" t="s">
-        <v>21</v>
+      <c r="I12" s="14" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>15</v>
@@ -1741,35 +1769,35 @@
         <v>1</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H14" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>33</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>15</v>
@@ -1791,12 +1819,12 @@
         <v>1</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>15</v>
@@ -1816,18 +1844,18 @@
         <v>1</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -1837,142 +1865,156 @@
         <v>2</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="12"/>
+      <c r="G18" s="7">
+        <v>0.5</v>
+      </c>
       <c r="H18" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>28</v>
+      <c r="I18" s="14" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="H19" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="H20" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
       <c r="I20" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="C21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="12"/>
+      <c r="G21" s="7">
+        <v>1</v>
+      </c>
       <c r="H21" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
-      </c>
-      <c r="I21" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="22" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H22" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="12"/>
+      <c r="G23" s="7">
+        <v>0.75</v>
+      </c>
       <c r="H23" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I23" s="5" t="s">
-        <v>50</v>
+      <c r="I23" s="14" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
@@ -1983,41 +2025,39 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I24" s="14" t="s">
-        <v>70</v>
+      <c r="I24" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="7">
-        <v>0.75</v>
-      </c>
+      <c r="G25" s="12"/>
       <c r="H25" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I25" s="5" t="s">
-        <v>48</v>
-      </c>
+      <c r="I25" s="5"/>
     </row>
     <row r="26" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="12"/>
@@ -2029,25 +2069,33 @@
     </row>
     <row r="27" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="12"/>
+      <c r="G27" s="7">
+        <v>1</v>
+      </c>
       <c r="H27" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
-      </c>
-      <c r="I27" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="28" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>11</v>
@@ -2061,23 +2109,23 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>1</v>
       </c>
-      <c r="I28" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="I28" s="5"/>
     </row>
     <row r="29" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
-      <c r="G29" s="12"/>
+      <c r="G29" s="7">
+        <v>0.75</v>
+      </c>
       <c r="H29" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
@@ -2086,30 +2134,30 @@
     </row>
     <row r="30" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H30" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>12</v>
@@ -2126,13 +2174,11 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>1</v>
       </c>
-      <c r="I31" s="5" t="s">
-        <v>57</v>
-      </c>
+      <c r="I31" s="5"/>
     </row>
     <row r="32" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
-        <v>117</v>
+        <v>52</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>12</v>
@@ -2149,14 +2195,16 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>1</v>
       </c>
-      <c r="I32" s="5"/>
-    </row>
-    <row r="33" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>11</v>
@@ -2170,16 +2218,14 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>1</v>
       </c>
-      <c r="I33" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>11</v>
@@ -2193,11 +2239,13 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>1</v>
       </c>
-      <c r="I34" s="5"/>
-    </row>
-    <row r="35" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I34" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>12</v>
@@ -2215,12 +2263,12 @@
         <v>1</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>12</v>
@@ -2237,16 +2285,14 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>1</v>
       </c>
-      <c r="I36" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>11</v>
@@ -2260,145 +2306,151 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>1</v>
       </c>
-      <c r="I37" s="5"/>
-    </row>
-    <row r="38" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I37" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
-      <c r="G38" s="7">
-        <v>1</v>
-      </c>
+      <c r="G38" s="12"/>
       <c r="H38" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>1</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I38" s="14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>83</v>
+        <v>156</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
-      <c r="G39" s="12"/>
+      <c r="G39" s="7">
+        <v>1</v>
+      </c>
       <c r="H39" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
-      </c>
-      <c r="I39" s="14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
+        <v>65</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
-      <c r="G40" s="12"/>
+      <c r="G40" s="7">
+        <v>0.75</v>
+      </c>
       <c r="H40" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I40" s="5"/>
-    </row>
-    <row r="41" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I40" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
       <c r="G41" s="7">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="H41" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
       <c r="G42" s="7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H42" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
-      <c r="G43" s="7">
-        <v>1</v>
-      </c>
+      <c r="G43" s="12"/>
       <c r="H43" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
@@ -2409,15 +2461,15 @@
       </c>
       <c r="I44" s="5"/>
     </row>
-    <row r="45" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
@@ -2428,15 +2480,15 @@
       </c>
       <c r="I45" s="5"/>
     </row>
-    <row r="46" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E46" s="9"/>
       <c r="F46" s="9"/>
@@ -2447,15 +2499,15 @@
       </c>
       <c r="I46" s="5"/>
     </row>
-    <row r="47" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
@@ -2466,15 +2518,15 @@
       </c>
       <c r="I47" s="5"/>
     </row>
-    <row r="48" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
@@ -2483,66 +2535,70 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I48" s="5"/>
-    </row>
-    <row r="49" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I48" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+    </row>
+    <row r="49" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
-      <c r="G49" s="12"/>
+      <c r="G49" s="7">
+        <v>0.75</v>
+      </c>
       <c r="H49" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I49" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
-      <c r="N49" s="5"/>
-    </row>
-    <row r="50" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I49" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E50" s="9"/>
       <c r="F50" s="9"/>
       <c r="G50" s="7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H50" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I50" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="51" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I50" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
@@ -2551,42 +2607,44 @@
       </c>
       <c r="H51" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="52" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I51" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E52" s="9"/>
       <c r="F52" s="9"/>
-      <c r="G52" s="12"/>
+      <c r="G52" s="7">
+        <v>1</v>
+      </c>
       <c r="H52" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="53" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E53" s="9"/>
       <c r="F53" s="9"/>
@@ -2597,130 +2655,132 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I53" s="14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="54" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I53" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
       <c r="G54" s="7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H54" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="55" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E55" s="9"/>
       <c r="F55" s="9"/>
-      <c r="G55" s="12"/>
+      <c r="G55" s="7">
+        <v>1</v>
+      </c>
       <c r="H55" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="56" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E56" s="9"/>
       <c r="F56" s="9"/>
       <c r="G56" s="7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H56" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="57" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="E57" s="9"/>
       <c r="F57" s="9"/>
-      <c r="G57" s="7">
-        <v>0.5</v>
-      </c>
+      <c r="G57" s="12"/>
       <c r="H57" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="58" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E58" s="9"/>
       <c r="F58" s="9"/>
-      <c r="G58" s="12"/>
+      <c r="G58" s="7">
+        <v>1</v>
+      </c>
       <c r="H58" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="59" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="5" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
@@ -2730,105 +2790,107 @@
         <v>2</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="60" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="E60" s="9"/>
       <c r="F60" s="9"/>
-      <c r="G60" s="12"/>
+      <c r="G60" s="7">
+        <v>1</v>
+      </c>
       <c r="H60" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="61" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E61" s="9"/>
       <c r="F61" s="9"/>
       <c r="G61" s="7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="H61" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="62" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="5" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E62" s="9"/>
       <c r="F62" s="9"/>
       <c r="G62" s="7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H62" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="63" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E63" s="9"/>
       <c r="F63" s="9"/>
       <c r="G63" s="7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="H63" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="64" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="5" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>11</v>
@@ -2843,108 +2905,108 @@
         <v>1</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="5" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E65" s="9"/>
       <c r="F65" s="9"/>
       <c r="G65" s="7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H65" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>1</v>
-      </c>
-      <c r="I65" s="5" t="s">
-        <v>146</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I65" s="5"/>
     </row>
     <row r="66" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="5" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E66" s="9"/>
       <c r="F66" s="9"/>
       <c r="G66" s="7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H66" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
-      </c>
-      <c r="I66" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="I66" s="5" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="67" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="5" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E67" s="9"/>
       <c r="F67" s="9"/>
       <c r="G67" s="7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H67" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
-      </c>
-      <c r="I67" s="5" t="s">
-        <v>135</v>
+        <v>1</v>
+      </c>
+      <c r="I67" s="14" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="68" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="5" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E68" s="9"/>
       <c r="F68" s="9"/>
       <c r="G68" s="7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H68" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
-      </c>
-      <c r="I68" s="14" t="s">
-        <v>134</v>
+        <v>1</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="69" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E69" s="9"/>
       <c r="F69" s="9"/>
@@ -2955,42 +3017,42 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I69" s="5" t="s">
-        <v>140</v>
-      </c>
+      <c r="I69" s="5"/>
     </row>
     <row r="70" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="5" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D70" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E70" s="9"/>
       <c r="F70" s="9"/>
-      <c r="G70" s="12"/>
+      <c r="G70" s="7">
+        <v>0.75</v>
+      </c>
       <c r="H70" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I70" s="5"/>
+      <c r="I70" s="5" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="71" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="5" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D71" s="5"/>
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
-      <c r="G71" s="7">
-        <v>0.25</v>
-      </c>
+      <c r="G71" s="12"/>
       <c r="H71" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
@@ -2999,38 +3061,42 @@
     </row>
     <row r="72" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="5" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E72" s="9"/>
       <c r="F72" s="9"/>
       <c r="G72" s="7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H72" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
     <row r="73" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="5" t="s">
-        <v>162</v>
+        <v>130</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D73" s="5"/>
+      <c r="D73" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E73" s="9"/>
       <c r="F73" s="9"/>
-      <c r="G73" s="12"/>
+      <c r="G73" s="7">
+        <v>0.75</v>
+      </c>
       <c r="H73" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
@@ -3039,10 +3105,10 @@
     </row>
     <row r="74" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="5" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>11</v>
@@ -3057,187 +3123,189 @@
         <v>1</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="75" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
       <c r="G75" s="7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="H75" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I75" s="5"/>
+      <c r="I75" s="5" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="76" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="5" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E76" s="9"/>
       <c r="F76" s="9"/>
       <c r="G76" s="7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="H76" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="5" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E77" s="9"/>
       <c r="F77" s="9"/>
       <c r="G77" s="7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H77" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="5" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E78" s="9"/>
       <c r="F78" s="9"/>
       <c r="G78" s="7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H78" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I78" s="5" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="79" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="5" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D79" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="E79" s="9"/>
       <c r="F79" s="9"/>
-      <c r="G79" s="12"/>
+      <c r="G79" s="7">
+        <v>1</v>
+      </c>
       <c r="H79" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
-      </c>
-      <c r="I79" s="5" t="s">
-        <v>160</v>
+        <v>1</v>
+      </c>
+      <c r="I79" s="14" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="80" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="5" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D80" s="5" t="s">
-        <v>36</v>
-      </c>
+      <c r="D80" s="5"/>
       <c r="E80" s="9"/>
       <c r="F80" s="9"/>
-      <c r="G80" s="7">
-        <v>1</v>
-      </c>
+      <c r="G80" s="12"/>
       <c r="H80" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I80" s="5" t="s">
-        <v>154</v>
-      </c>
+      <c r="I80" s="5"/>
     </row>
     <row r="81" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D81" s="5"/>
       <c r="E81" s="9"/>
       <c r="F81" s="9"/>
-      <c r="G81" s="7">
-        <v>0.5</v>
-      </c>
+      <c r="G81" s="12"/>
       <c r="H81" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I81" s="5" t="s">
-        <v>159</v>
-      </c>
+      <c r="I81" s="5"/>
     </row>
     <row r="82" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="5" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D82" s="5"/>
+      <c r="D82" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="E82" s="9"/>
       <c r="F82" s="9"/>
-      <c r="G82" s="12"/>
+      <c r="G82" s="7">
+        <v>1</v>
+      </c>
       <c r="H82" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I82" s="5"/>
     </row>
     <row r="83" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
+        <v>164</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="E83" s="9"/>
       <c r="F83" s="9"/>
       <c r="G83" s="12"/>
@@ -3245,33 +3313,161 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I83" s="5"/>
+      <c r="I83" s="5" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="84" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="E84" s="9"/>
       <c r="F84" s="9"/>
-      <c r="G84" s="7">
+      <c r="G84" s="12"/>
+      <c r="H84" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="12"/>
+      <c r="H85" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
+      <c r="G86" s="12"/>
+      <c r="H86" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I86" s="5"/>
+    </row>
+    <row r="87" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="12"/>
+      <c r="H87" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I87" s="5"/>
+    </row>
+    <row r="88" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="7">
         <v>0.75</v>
       </c>
-      <c r="H84" s="13">
-        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
-      </c>
-      <c r="I84" s="5"/>
+      <c r="H88" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I88" s="5"/>
+    </row>
+    <row r="89" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="12"/>
+      <c r="H89" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I89" s="5"/>
+    </row>
+    <row r="90" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="12"/>
+      <c r="H90" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I90" s="5"/>
+    </row>
+    <row r="91" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9"/>
+      <c r="G91" s="12"/>
+      <c r="H91" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I91" s="5"/>
+    </row>
+    <row r="92" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="H92" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I92" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G5:G84">
-    <cfRule type="dataBar" priority="59">
+  <conditionalFormatting sqref="G5:G92">
+    <cfRule type="dataBar" priority="64">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3285,17 +3481,17 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" sqref="G5:G84">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly you need to select a choice from the drop down list. But you can still use what you entered by clicking Yes." sqref="B21 D5:D92">
+      <formula1>"Non commencée,En cours de réalisation, Différé, Terminée"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="G5:G92">
       <formula1>"0%,25%,50%,75%,100%"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Whoops" sqref="C5:C84">
+    <dataValidation type="list" allowBlank="1" errorTitle="Whoops" sqref="C5:C92">
       <formula1>"Basse, Normale, Élevée"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly, your Due Date needs to be greater than or equal to the Start Date." sqref="F5:F84">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly, your Due Date needs to be greater than or equal to the Start Date." sqref="F5:F92">
       <formula1>F5&gt;=E5</formula1>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly you need to select a choice from the drop down list. But you can still use what you entered by clicking Yes." sqref="D5:D84 B22">
-      <formula1>"Non commencée,En cours de réalisation, Différé, Terminée"</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
@@ -3321,10 +3517,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G5:G84</xm:sqref>
+          <xm:sqref>G5:G92</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="60" id="{61976558-4184-4BD1-B78A-DCBE6FDA3BC9}">
+          <x14:cfRule type="iconSet" priority="66" id="{61976558-4184-4BD1-B78A-DCBE6FDA3BC9}">
             <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -3340,7 +3536,7 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>H5:H84</xm:sqref>
+          <xm:sqref>H5:H92</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3366,28 +3562,28 @@
   <sheetData>
     <row r="1" spans="3:11" s="15" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
       <c r="C1" s="15" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="3:11" x14ac:dyDescent="0.25">
@@ -3955,7 +4151,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C24">
         <v>40</v>
@@ -4066,7 +4262,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C30">
         <v>40</v>
@@ -4126,7 +4322,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C33">
         <v>40</v>
@@ -4261,7 +4457,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C39">
         <v>40</v>
@@ -4372,7 +4568,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added distance control before moving
</commit_message>
<xml_diff>
--- a/ProjectDocumention/PlanDeConvergenceIntegration.xlsx
+++ b/ProjectDocumention/PlanDeConvergenceIntegration.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="28860" yWindow="0" windowWidth="19200" windowHeight="11265"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="182">
   <si>
     <r>
       <rPr>
@@ -642,13 +642,37 @@
     <t>Etendre apprentissage echo au salon &amp; etendre zonexy</t>
   </si>
   <si>
-    <t>Tester echolocalisation avec ML rotation virtuelele</t>
-  </si>
-  <si>
     <t>Avant  move verifier faisabilite avec echo</t>
   </si>
   <si>
     <t>Avant rotation verifier faisabilite avec echo</t>
+  </si>
+  <si>
+    <t>Tester echolocalisation avec ML rotation virtuelle</t>
+  </si>
+  <si>
+    <t>Traiter le cas move impossible dans octave</t>
+  </si>
+  <si>
+    <t>remonter min echo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revoir le calcul du path </t>
+  </si>
+  <si>
+    <t>cf cours EDX (soit potentiel ou chemin predetermine et utiliser le astar pour rejonidre le point le + proche predefini)</t>
+  </si>
+  <si>
+    <t>Traiter le cas localisation theorique impossible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revoir Octave avec un Objet robot </t>
+  </si>
+  <si>
+    <t>Opitmiser le move particles</t>
+  </si>
+  <si>
+    <t>Distinguer les cas roue stopped et decalge de speed</t>
   </si>
 </sst>
 </file>
@@ -658,7 +682,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
@@ -722,6 +746,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -784,7 +814,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -838,6 +868,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1248,8 +1281,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Liste_de_tâches" displayName="Liste_de_tâches" ref="B4:I92" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B4:I92"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Liste_de_tâches" displayName="Liste_de_tâches" ref="B4:I98" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B4:I98"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Tâche" dataDxfId="7"/>
     <tableColumn id="3" name="Priorité " dataDxfId="6"/>
@@ -1512,10 +1545,10 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:N92"/>
+  <dimension ref="B1:N98"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G92" sqref="G92"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1577,7 +1610,7 @@
       </c>
       <c r="F5" s="8">
         <f ca="1">TODAY()-1</f>
-        <v>42844</v>
+        <v>42859</v>
       </c>
       <c r="G5" s="4">
         <v>1</v>
@@ -3383,7 +3416,7 @@
     </row>
     <row r="88" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C88" s="5" t="s">
         <v>12</v>
@@ -3400,7 +3433,9 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I88" s="5"/>
+      <c r="I88" s="18" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="89" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="5" t="s">
@@ -3434,7 +3469,7 @@
     </row>
     <row r="91" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
@@ -3449,10 +3484,12 @@
     </row>
     <row r="92" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C92" s="5"/>
-      <c r="D92" s="5"/>
+      <c r="D92" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E92" s="9"/>
       <c r="F92" s="9"/>
       <c r="G92" s="7">
@@ -3464,9 +3501,109 @@
       </c>
       <c r="I92" s="5"/>
     </row>
+    <row r="93" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="H93" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I93" s="5"/>
+    </row>
+    <row r="94" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="9"/>
+      <c r="G94" s="12"/>
+      <c r="H94" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I94" s="5"/>
+    </row>
+    <row r="95" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
+      <c r="G95" s="12"/>
+      <c r="H95" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I95" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="96" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="9"/>
+      <c r="G96" s="12"/>
+      <c r="H96" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I96" s="5"/>
+    </row>
+    <row r="97" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="9"/>
+      <c r="G97" s="12"/>
+      <c r="H97" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I97" s="5"/>
+    </row>
+    <row r="98" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E98" s="9"/>
+      <c r="F98" s="9"/>
+      <c r="G98" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="H98" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I98" s="5"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G5:G92">
+  <conditionalFormatting sqref="G5:G98">
     <cfRule type="dataBar" priority="64">
       <dataBar>
         <cfvo type="min"/>
@@ -3481,16 +3618,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly you need to select a choice from the drop down list. But you can still use what you entered by clicking Yes." sqref="B21 D5:D92">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly you need to select a choice from the drop down list. But you can still use what you entered by clicking Yes." sqref="B21 D5:D98">
       <formula1>"Non commencée,En cours de réalisation, Différé, Terminée"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G5:G92">
+    <dataValidation type="list" allowBlank="1" sqref="G5:G98">
       <formula1>"0%,25%,50%,75%,100%"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Whoops" sqref="C5:C92">
+    <dataValidation type="list" allowBlank="1" errorTitle="Whoops" sqref="C5:C98">
       <formula1>"Basse, Normale, Élevée"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly, your Due Date needs to be greater than or equal to the Start Date." sqref="F5:F92">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly, your Due Date needs to be greater than or equal to the Start Date." sqref="F5:F98">
       <formula1>F5&gt;=E5</formula1>
     </dataValidation>
   </dataValidations>
@@ -3517,7 +3654,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G5:G92</xm:sqref>
+          <xm:sqref>G5:G98</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="66" id="{61976558-4184-4BD1-B78A-DCBE6FDA3BC9}">
@@ -3536,7 +3673,7 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>H5:H92</xm:sqref>
+          <xm:sqref>H5:H98</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
4 voltages monitoring added
</commit_message>
<xml_diff>
--- a/ProjectDocumention/PlanDeConvergenceIntegration.xlsx
+++ b/ProjectDocumention/PlanDeConvergenceIntegration.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="213">
   <si>
     <r>
       <rPr>
@@ -700,6 +700,72 @@
   </si>
   <si>
     <t xml:space="preserve">pour tunning dynamique </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tester debuger le ping front </t>
+  </si>
+  <si>
+    <t>Remplacer le servo moteur pour eviter tremblements</t>
+  </si>
+  <si>
+    <t>Faire releve des pings en approche de portes</t>
+  </si>
+  <si>
+    <t>Distinguer echo 0 de echo max</t>
+  </si>
+  <si>
+    <t>surveiller le non decalage position encodeur VS roue</t>
+  </si>
+  <si>
+    <t>via marque noire</t>
+  </si>
+  <si>
+    <t>Monitorer l alim des moteurs (avant et apres regulateur)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stocker en BD les tensions </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verifier / modifier le wait apres atteinte seuil encodeur pour prendre en compte la fin de mouvement </t>
+  </si>
+  <si>
+    <t>Developper une fonction octave graph compare de 2 trajectoires avec heading</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ApShowComparedStep(apRobot,det,actualPositions,"blue cyan: determined -- black red: actual")</t>
+  </si>
+  <si>
+    <t>Java ne pas enregistrer les records scan recus en double</t>
+  </si>
+  <si>
+    <t>ajout d un timer dans la loop en lieu et place du delay</t>
+  </si>
+  <si>
+    <t>pour identifier les pbs d alimentation via une non montee du signal - a traiter via librairie NewPing</t>
+  </si>
+  <si>
+    <t>Constituer un dossier de maintenance (procedure outils checklist,,,)</t>
+  </si>
+  <si>
+    <t>semble irregulier VS ping back &gt;&gt; apres analyse SRF-05 return 0 aux environs de 3m (la doc parle de 4m) Front et Back sont similaires</t>
+  </si>
+  <si>
+    <t>Developper une fonction test echo</t>
+  </si>
+  <si>
+    <t>LoopPingFB,m + MySql repondent au besoin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Etendre la carto au couloir et 1ere partie du salon </t>
+  </si>
+  <si>
+    <t>a faire les jeux de tests</t>
+  </si>
+  <si>
+    <t>to be checked</t>
+  </si>
+  <si>
+    <t>a valider en reel</t>
   </si>
 </sst>
 </file>
@@ -777,7 +843,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -908,7 +974,7 @@
     <cellStyle name="Titre 2" xfId="4" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Titre 3" xfId="5" builtinId="18" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="26">
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1116,8 +1182,34 @@
         </vertical>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
-  <tableStyles count="2" defaultTableStyle="To Do List" defaultPivotStyle="PivotStyleMedium13">
+  <tableStyles count="3" defaultTableStyle="To Do List" defaultPivotStyle="PivotStyleMedium13">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="25"/>
+      <tableStyleElement type="headerRow" dxfId="24"/>
+    </tableStyle>
     <tableStyle name="To Do List" pivot="0" count="3">
       <tableStyleElement type="wholeTable" dxfId="23"/>
       <tableStyleElement type="headerRow" dxfId="22"/>
@@ -1308,8 +1400,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Liste_de_tâches" displayName="Liste_de_tâches" ref="B4:I103" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B4:I103"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Liste_de_tâches" displayName="Liste_de_tâches" ref="B4:I116" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B4:I116"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Tâche" dataDxfId="7"/>
     <tableColumn id="3" name="Priorité " dataDxfId="6"/>
@@ -1572,10 +1664,10 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:N103"/>
+  <dimension ref="B1:N116"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C100" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I107" sqref="I107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1637,7 +1729,7 @@
       </c>
       <c r="F5" s="8">
         <f ca="1">TODAY()-1</f>
-        <v>42926</v>
+        <v>42942</v>
       </c>
       <c r="G5" s="4">
         <v>1</v>
@@ -2612,16 +2704,16 @@
         <v>12</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
       <c r="G49" s="7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H49" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I49" s="14" t="s">
         <v>103</v>
@@ -3489,12 +3581,12 @@
       </c>
       <c r="C90" s="5"/>
       <c r="D90" s="5" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E90" s="9"/>
       <c r="F90" s="9"/>
       <c r="G90" s="7">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H90" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
@@ -3739,10 +3831,261 @@
         <v>190</v>
       </c>
     </row>
+    <row r="104" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E104" s="9"/>
+      <c r="F104" s="9"/>
+      <c r="G104" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="H104" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I104" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="9"/>
+      <c r="F105" s="9"/>
+      <c r="G105" s="12"/>
+      <c r="H105" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I105" s="5"/>
+    </row>
+    <row r="106" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="9"/>
+      <c r="F106" s="9"/>
+      <c r="G106" s="12"/>
+      <c r="H106" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I106" s="5"/>
+    </row>
+    <row r="107" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E107" s="9"/>
+      <c r="F107" s="9"/>
+      <c r="G107" s="12"/>
+      <c r="H107" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I107" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C108" s="5"/>
+      <c r="D108" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E108" s="9"/>
+      <c r="F108" s="9"/>
+      <c r="G108" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="H108" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I108" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E109" s="9"/>
+      <c r="F109" s="9"/>
+      <c r="G109" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="H109" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I109" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E110" s="9"/>
+      <c r="F110" s="9"/>
+      <c r="G110" s="7">
+        <v>1</v>
+      </c>
+      <c r="H110" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>1</v>
+      </c>
+      <c r="I110" s="5"/>
+    </row>
+    <row r="111" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B111" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C111" s="5"/>
+      <c r="D111" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E111" s="9"/>
+      <c r="F111" s="9"/>
+      <c r="G111" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="H111" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I111" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="112" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C112" s="5"/>
+      <c r="D112" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E112" s="9"/>
+      <c r="F112" s="9"/>
+      <c r="G112" s="7">
+        <v>1</v>
+      </c>
+      <c r="H112" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>1</v>
+      </c>
+      <c r="I112" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="113" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C113" s="5"/>
+      <c r="D113" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E113" s="9"/>
+      <c r="F113" s="9"/>
+      <c r="G113" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="H113" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I113" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5"/>
+      <c r="E114" s="9"/>
+      <c r="F114" s="9"/>
+      <c r="G114" s="12"/>
+      <c r="H114" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I114" s="5"/>
+    </row>
+    <row r="115" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B115" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C115" s="5"/>
+      <c r="D115" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E115" s="9"/>
+      <c r="F115" s="9"/>
+      <c r="G115" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="H115" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I115" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="116" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C116" s="5"/>
+      <c r="D116" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E116" s="9"/>
+      <c r="F116" s="9"/>
+      <c r="G116" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="H116" s="13">
+        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="I116" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G5:G103">
-    <cfRule type="dataBar" priority="64">
+  <conditionalFormatting sqref="G5:G116">
+    <cfRule type="dataBar" priority="67">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3756,16 +4099,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly you need to select a choice from the drop down list. But you can still use what you entered by clicking Yes." sqref="B21 D5:D103">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly you need to select a choice from the drop down list. But you can still use what you entered by clicking Yes." sqref="B21 D5:D116">
       <formula1>"Non commencée,En cours de réalisation, Différé, Terminée"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G5:G103">
+    <dataValidation type="list" allowBlank="1" sqref="G5:G116">
       <formula1>"0%,25%,50%,75%,100%"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Whoops" sqref="C5:C103">
+    <dataValidation type="list" allowBlank="1" errorTitle="Whoops" sqref="C5:C116">
       <formula1>"Basse, Normale, Élevée"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly, your Due Date needs to be greater than or equal to the Start Date." sqref="F5:F103">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly, your Due Date needs to be greater than or equal to the Start Date." sqref="F5:F116">
       <formula1>F5&gt;=E5</formula1>
     </dataValidation>
   </dataValidations>
@@ -3792,10 +4135,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G5:G103</xm:sqref>
+          <xm:sqref>G5:G116</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="66" id="{61976558-4184-4BD1-B78A-DCBE6FDA3BC9}">
+          <x14:cfRule type="iconSet" priority="68" id="{61976558-4184-4BD1-B78A-DCBE6FDA3BC9}">
             <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -3811,7 +4154,7 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>H5:H103</xm:sqref>
+          <xm:sqref>H5:H116</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
stopping encoders & voltage threshold modified
</commit_message>
<xml_diff>
--- a/ProjectDocumention/PlanDeConvergenceIntegration.xlsx
+++ b/ProjectDocumention/PlanDeConvergenceIntegration.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="219">
   <si>
     <r>
       <rPr>
@@ -621,9 +621,6 @@
     <t>Revoir la façon de determiner le path (type Voronoi graph ou potentiel field ou probabilistic road map planner ?)</t>
   </si>
   <si>
-    <t>Rechercer des bibliothques Octave pour accroitre performance de l analyse  echo (cf biblio python)</t>
-  </si>
-  <si>
     <t>dans Octave traduire les coordonnees du robot sous forme de matrice (x,y,theta)</t>
   </si>
   <si>
@@ -648,12 +645,6 @@
     <t>Traiter le cas move impossible dans octave</t>
   </si>
   <si>
-    <t>remonter min echo</t>
-  </si>
-  <si>
-    <t>Traiter le cas localisation theorique impossible</t>
-  </si>
-  <si>
     <t xml:space="preserve">Revoir Octave avec un Objet robot </t>
   </si>
   <si>
@@ -675,9 +666,6 @@
     <t>suivant chemin predefini</t>
   </si>
   <si>
-    <t>Developper une fonction franchissement de porte</t>
-  </si>
-  <si>
     <t xml:space="preserve">sur base de scan intensifs completes de mesures directes </t>
   </si>
   <si>
@@ -705,9 +693,6 @@
     <t>Remplacer le servo moteur pour eviter tremblements</t>
   </si>
   <si>
-    <t>Faire releve des pings en approche de portes</t>
-  </si>
-  <si>
     <t>Distinguer echo 0 de echo max</t>
   </si>
   <si>
@@ -775,6 +760,30 @@
   </si>
   <si>
     <t>Utiliser le gyroscope pour affiner le mouvement rectiligne (PID ?)</t>
+  </si>
+  <si>
+    <t>via octave</t>
+  </si>
+  <si>
+    <t>Rechercher des bibliothques Octave pour accroitre performance de l analyse  echo (cf biblio python)</t>
+  </si>
+  <si>
+    <t>reste à valider le cas echo à 0</t>
+  </si>
+  <si>
+    <t>lancer une localisation fine ?</t>
+  </si>
+  <si>
+    <t>Developper une fonction franchissement de passages delicats</t>
+  </si>
+  <si>
+    <t>Faire releve des pings pour localisation fine</t>
+  </si>
+  <si>
+    <t>commencer par approche des portes</t>
+  </si>
+  <si>
+    <t>type porte  &gt;&gt; appliquer des consignes liees à une localisation</t>
   </si>
 </sst>
 </file>
@@ -1409,8 +1418,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Liste_de_tâches" displayName="Liste_de_tâches" ref="B4:I118" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B4:I118"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Liste_de_tâches" displayName="Liste_de_tâches" ref="B4:I117" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B4:I117">
+    <filterColumn colId="2">
+      <filters blank="1">
+        <filter val="Différé"/>
+        <filter val="En cours de réalisation"/>
+        <filter val="Non commencée"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" name="Tâche" dataDxfId="7"/>
     <tableColumn id="3" name="Priorité " dataDxfId="6"/>
@@ -1673,10 +1690,10 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:N118"/>
+  <dimension ref="B1:N117"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I99" sqref="I99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1723,7 +1740,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
         <v>20</v>
       </c>
@@ -1738,7 +1755,7 @@
       </c>
       <c r="F5" s="8">
         <f ca="1">TODAY()-1</f>
-        <v>42943</v>
+        <v>42944</v>
       </c>
       <c r="G5" s="4">
         <v>1</v>
@@ -1749,7 +1766,7 @@
       </c>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>34</v>
       </c>
@@ -1770,7 +1787,7 @@
       </c>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>30</v>
       </c>
@@ -1793,7 +1810,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>14</v>
       </c>
@@ -1862,7 +1879,7 @@
       </c>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
@@ -1889,7 +1906,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>21</v>
       </c>
@@ -1910,7 +1927,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>22</v>
       </c>
@@ -1933,7 +1950,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>23</v>
       </c>
@@ -1956,7 +1973,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>26</v>
       </c>
@@ -1983,7 +2000,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>24</v>
       </c>
@@ -2098,7 +2115,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>39</v>
       </c>
@@ -2121,7 +2138,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>40</v>
       </c>
@@ -2228,7 +2245,7 @@
       </c>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>47</v>
       </c>
@@ -2251,7 +2268,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>49</v>
       </c>
@@ -2272,7 +2289,7 @@
       </c>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>53</v>
       </c>
@@ -2293,7 +2310,7 @@
       </c>
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>50</v>
       </c>
@@ -2316,7 +2333,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>106</v>
       </c>
@@ -2337,7 +2354,7 @@
       </c>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>52</v>
       </c>
@@ -2360,7 +2377,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>54</v>
       </c>
@@ -2381,7 +2398,7 @@
       </c>
       <c r="I33" s="5"/>
     </row>
-    <row r="34" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>55</v>
       </c>
@@ -2404,7 +2421,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="35" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>56</v>
       </c>
@@ -2427,7 +2444,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>57</v>
       </c>
@@ -2448,7 +2465,7 @@
       </c>
       <c r="I36" s="5"/>
     </row>
-    <row r="37" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>58</v>
       </c>
@@ -2492,7 +2509,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>156</v>
       </c>
@@ -2559,7 +2576,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>68</v>
       </c>
@@ -2705,7 +2722,7 @@
       <c r="M48" s="5"/>
       <c r="N48" s="5"/>
     </row>
-    <row r="49" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
         <v>162</v>
       </c>
@@ -2751,7 +2768,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>78</v>
       </c>
@@ -2774,7 +2791,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>79</v>
       </c>
@@ -2820,7 +2837,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>83</v>
       </c>
@@ -2843,7 +2860,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="55" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
         <v>84</v>
       </c>
@@ -2866,7 +2883,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
         <v>87</v>
       </c>
@@ -2910,7 +2927,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="5" t="s">
         <v>107</v>
       </c>
@@ -2954,7 +2971,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="60" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="s">
         <v>110</v>
       </c>
@@ -2977,7 +2994,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="61" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
         <v>115</v>
       </c>
@@ -3000,7 +3017,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="62" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="5" t="s">
         <v>113</v>
       </c>
@@ -3023,7 +3040,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="s">
         <v>116</v>
       </c>
@@ -3046,7 +3063,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="64" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="5" t="s">
         <v>118</v>
       </c>
@@ -3090,7 +3107,7 @@
       </c>
       <c r="I65" s="5"/>
     </row>
-    <row r="66" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="5" t="s">
         <v>120</v>
       </c>
@@ -3113,7 +3130,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="67" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="5" t="s">
         <v>121</v>
       </c>
@@ -3136,7 +3153,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="5" t="s">
         <v>149</v>
       </c>
@@ -3159,7 +3176,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="s">
         <v>128</v>
       </c>
@@ -3167,20 +3184,20 @@
         <v>12</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E69" s="9"/>
       <c r="F69" s="9"/>
       <c r="G69" s="7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="H69" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I69" s="5"/>
     </row>
-    <row r="70" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="5" t="s">
         <v>125</v>
       </c>
@@ -3188,22 +3205,22 @@
         <v>12</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E70" s="9"/>
       <c r="F70" s="9"/>
       <c r="G70" s="7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H70" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I70" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="71" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="5" t="s">
         <v>148</v>
       </c>
@@ -3224,7 +3241,7 @@
       </c>
       <c r="I71" s="5"/>
     </row>
-    <row r="72" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="5" t="s">
         <v>129</v>
       </c>
@@ -3268,7 +3285,7 @@
       </c>
       <c r="I73" s="5"/>
     </row>
-    <row r="74" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="5" t="s">
         <v>131</v>
       </c>
@@ -3291,7 +3308,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="75" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
         <v>135</v>
       </c>
@@ -3299,22 +3316,22 @@
         <v>12</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
       <c r="G75" s="7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H75" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I75" s="5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="76" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="5" t="s">
         <v>137</v>
       </c>
@@ -3322,22 +3339,22 @@
         <v>12</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E76" s="9"/>
       <c r="F76" s="9"/>
       <c r="G76" s="7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H76" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I76" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="77" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="5" t="s">
         <v>139</v>
       </c>
@@ -3360,7 +3377,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="78" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="5" t="s">
         <v>142</v>
       </c>
@@ -3383,7 +3400,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="79" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="5" t="s">
         <v>144</v>
       </c>
@@ -3430,17 +3447,23 @@
       <c r="C81" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D81" s="5"/>
+      <c r="D81" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E81" s="9"/>
       <c r="F81" s="9"/>
-      <c r="G81" s="12"/>
+      <c r="G81" s="7">
+        <v>0.25</v>
+      </c>
       <c r="H81" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I81" s="5"/>
-    </row>
-    <row r="82" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I81" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="5" t="s">
         <v>150</v>
       </c>
@@ -3481,12 +3504,12 @@
         <v>2</v>
       </c>
       <c r="I83" s="5" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="84" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="5" t="s">
-        <v>164</v>
+        <v>212</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>10</v>
@@ -3503,9 +3526,9 @@
       </c>
       <c r="I84" s="5"/>
     </row>
-    <row r="85" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="5" t="s">
@@ -3521,12 +3544,12 @@
         <v>1</v>
       </c>
       <c r="I85" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="86" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C86" s="5"/>
       <c r="D86" s="5" t="s">
@@ -3545,10 +3568,12 @@
     </row>
     <row r="87" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C87" s="5"/>
-      <c r="D87" s="5"/>
+      <c r="D87" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="E87" s="9"/>
       <c r="F87" s="9"/>
       <c r="G87" s="12"/>
@@ -3560,7 +3585,7 @@
     </row>
     <row r="88" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C88" s="5" t="s">
         <v>12</v>
@@ -3578,15 +3603,17 @@
         <v>2</v>
       </c>
       <c r="I88" s="18" t="s">
-        <v>173</v>
+        <v>213</v>
       </c>
     </row>
     <row r="89" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
+      <c r="D89" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="E89" s="9"/>
       <c r="F89" s="9"/>
       <c r="G89" s="12"/>
@@ -3594,11 +3621,13 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I89" s="5"/>
+      <c r="I89" s="5" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="90" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C90" s="5"/>
       <c r="D90" s="5" t="s">
@@ -3617,10 +3646,12 @@
     </row>
     <row r="91" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C91" s="5"/>
-      <c r="D91" s="5"/>
+      <c r="D91" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E91" s="9"/>
       <c r="F91" s="9"/>
       <c r="G91" s="12"/>
@@ -3632,7 +3663,7 @@
     </row>
     <row r="92" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="5" t="s">
@@ -3651,7 +3682,7 @@
     </row>
     <row r="93" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C93" s="5"/>
       <c r="D93" s="5" t="s">
@@ -3670,22 +3701,28 @@
     </row>
     <row r="94" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
+      <c r="D94" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E94" s="9"/>
       <c r="F94" s="9"/>
-      <c r="G94" s="12"/>
+      <c r="G94" s="7">
+        <v>0.75</v>
+      </c>
       <c r="H94" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I94" s="5"/>
+      <c r="I94" s="5" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="95" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="5" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C95" s="5"/>
       <c r="D95" s="5" t="s">
@@ -3694,46 +3731,46 @@
       <c r="E95" s="9"/>
       <c r="F95" s="9"/>
       <c r="G95" s="7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H95" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
       <c r="I95" s="5" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="96" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C96" s="5"/>
       <c r="D96" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E96" s="9"/>
       <c r="F96" s="9"/>
-      <c r="G96" s="7">
-        <v>1</v>
-      </c>
+      <c r="G96" s="12"/>
       <c r="H96" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I96" s="5" t="s">
-        <v>187</v>
-      </c>
+      <c r="I96" s="5"/>
     </row>
     <row r="97" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="5" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C97" s="5"/>
-      <c r="D97" s="5"/>
+      <c r="D97" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E97" s="9"/>
       <c r="F97" s="9"/>
-      <c r="G97" s="12"/>
+      <c r="G97" s="7">
+        <v>0.5</v>
+      </c>
       <c r="H97" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
@@ -3742,7 +3779,7 @@
     </row>
     <row r="98" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C98" s="5"/>
       <c r="D98" s="5" t="s">
@@ -3761,29 +3798,31 @@
     </row>
     <row r="99" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
-        <v>180</v>
+        <v>215</v>
       </c>
       <c r="C99" s="5"/>
       <c r="D99" s="5" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E99" s="9"/>
       <c r="F99" s="9"/>
-      <c r="G99" s="7">
-        <v>0.5</v>
-      </c>
+      <c r="G99" s="12"/>
       <c r="H99" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I99" s="5"/>
+      <c r="I99" s="5" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="100" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C100" s="5"/>
-      <c r="D100" s="5"/>
+      <c r="D100" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="E100" s="9"/>
       <c r="F100" s="9"/>
       <c r="G100" s="12"/>
@@ -3791,28 +3830,34 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I100" s="5"/>
-    </row>
-    <row r="101" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I100" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C101" s="5"/>
-      <c r="D101" s="5"/>
+      <c r="D101" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="E101" s="9"/>
       <c r="F101" s="9"/>
-      <c r="G101" s="12"/>
+      <c r="G101" s="7">
+        <v>1</v>
+      </c>
       <c r="H101" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I101" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="102" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C102" s="5"/>
       <c r="D102" s="5" t="s">
@@ -3828,12 +3873,12 @@
         <v>1</v>
       </c>
       <c r="I102" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="103" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C103" s="5"/>
       <c r="D103" s="5" t="s">
@@ -3849,51 +3894,55 @@
         <v>1</v>
       </c>
       <c r="I103" s="5" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
     </row>
     <row r="104" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C104" s="5"/>
       <c r="D104" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E104" s="9"/>
       <c r="F104" s="9"/>
-      <c r="G104" s="7">
-        <v>0.75</v>
-      </c>
+      <c r="G104" s="12"/>
       <c r="H104" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I104" s="5" t="s">
-        <v>205</v>
-      </c>
+      <c r="I104" s="5"/>
     </row>
     <row r="105" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="5" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
       <c r="C105" s="5"/>
-      <c r="D105" s="5"/>
+      <c r="D105" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E105" s="9"/>
       <c r="F105" s="9"/>
-      <c r="G105" s="12"/>
+      <c r="G105" s="7">
+        <v>0.5</v>
+      </c>
       <c r="H105" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I105" s="5"/>
+      <c r="I105" s="5" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="106" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C106" s="5"/>
-      <c r="D106" s="5"/>
+      <c r="D106" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E106" s="9"/>
       <c r="F106" s="9"/>
       <c r="G106" s="12"/>
@@ -3901,30 +3950,34 @@
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I106" s="5"/>
+      <c r="I106" s="5" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="107" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="5" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C107" s="5"/>
       <c r="D107" s="5" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E107" s="9"/>
       <c r="F107" s="9"/>
-      <c r="G107" s="12"/>
+      <c r="G107" s="7">
+        <v>0.25</v>
+      </c>
       <c r="H107" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
       <c r="I107" s="5" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
     </row>
     <row r="108" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C108" s="5"/>
       <c r="D108" s="5" t="s">
@@ -3933,137 +3986,139 @@
       <c r="E108" s="9"/>
       <c r="F108" s="9"/>
       <c r="G108" s="7">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="H108" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
       <c r="I108" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="109" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="5" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C109" s="5"/>
       <c r="D109" s="5" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E109" s="9"/>
       <c r="F109" s="9"/>
       <c r="G109" s="7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H109" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
-      </c>
-      <c r="I109" s="5" t="s">
-        <v>211</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I109" s="5"/>
     </row>
     <row r="110" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="5" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C110" s="5"/>
       <c r="D110" s="5" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E110" s="9"/>
       <c r="F110" s="9"/>
       <c r="G110" s="7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="H110" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>1</v>
-      </c>
-      <c r="I110" s="5"/>
-    </row>
-    <row r="111" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I110" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C111" s="5"/>
       <c r="D111" s="5" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E111" s="9"/>
       <c r="F111" s="9"/>
       <c r="G111" s="7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H111" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I111" s="5" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="112" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C112" s="5"/>
       <c r="D112" s="5" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E112" s="9"/>
       <c r="F112" s="9"/>
       <c r="G112" s="7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="H112" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I112" s="5" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="113" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C113" s="5"/>
       <c r="D113" s="5" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E113" s="9"/>
       <c r="F113" s="9"/>
-      <c r="G113" s="7">
-        <v>0.75</v>
-      </c>
+      <c r="G113" s="12"/>
       <c r="H113" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I113" s="5" t="s">
-        <v>210</v>
-      </c>
+      <c r="I113" s="5"/>
     </row>
     <row r="114" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C114" s="5"/>
-      <c r="D114" s="5"/>
+      <c r="D114" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E114" s="9"/>
       <c r="F114" s="9"/>
-      <c r="G114" s="12"/>
+      <c r="G114" s="7">
+        <v>0.75</v>
+      </c>
       <c r="H114" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I114" s="5"/>
+      <c r="I114" s="5" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="115" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C115" s="5"/>
       <c r="D115" s="5" t="s">
@@ -4072,45 +4127,43 @@
       <c r="E115" s="9"/>
       <c r="F115" s="9"/>
       <c r="G115" s="7">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="H115" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
       <c r="I115" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="116" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C116" s="5"/>
+        <v>209</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D116" s="5" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E116" s="9"/>
       <c r="F116" s="9"/>
-      <c r="G116" s="7">
-        <v>0.5</v>
-      </c>
+      <c r="G116" s="12"/>
       <c r="H116" s="13">
         <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="I116" s="5" t="s">
-        <v>209</v>
-      </c>
+      <c r="I116" s="5"/>
     </row>
     <row r="117" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="C117" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D117" s="5"/>
+        <v>210</v>
+      </c>
+      <c r="C117" s="5"/>
+      <c r="D117" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="E117" s="9"/>
       <c r="F117" s="9"/>
       <c r="G117" s="12"/>
@@ -4120,25 +4173,10 @@
       </c>
       <c r="I117" s="5"/>
     </row>
-    <row r="118" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B118" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="C118" s="5"/>
-      <c r="D118" s="5"/>
-      <c r="E118" s="9"/>
-      <c r="F118" s="9"/>
-      <c r="G118" s="12"/>
-      <c r="H118" s="13">
-        <f ca="1">IF(AND(Liste_de_tâches[[#This Row],[État ]]="Terminée",Liste_de_tâches[[#This Row],[% achevé]]=1),1,IF(ISBLANK(Liste_de_tâches[[#This Row],[Échéance ]]),2,IF(AND(Liste_de_tâches[[#This Row],[État ]]&lt;&gt;"Terminée",TODAY()&gt;Liste_de_tâches[[#This Row],[Échéance ]]),3,2)))</f>
-        <v>2</v>
-      </c>
-      <c r="I118" s="5"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G5:G118">
-    <cfRule type="dataBar" priority="67">
+  <conditionalFormatting sqref="G5:G117">
+    <cfRule type="dataBar" priority="69">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4152,16 +4190,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly you need to select a choice from the drop down list. But you can still use what you entered by clicking Yes." sqref="B21 D5:D118">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly you need to select a choice from the drop down list. But you can still use what you entered by clicking Yes." sqref="B21 D5:D117">
       <formula1>"Non commencée,En cours de réalisation, Différé, Terminée"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G5:G118">
+    <dataValidation type="list" allowBlank="1" sqref="G5:G117">
       <formula1>"0%,25%,50%,75%,100%"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Whoops" sqref="C5:C118">
+    <dataValidation type="list" allowBlank="1" errorTitle="Whoops" sqref="C5:C117">
       <formula1>"Basse, Normale, Élevée"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly, your Due Date needs to be greater than or equal to the Start Date." sqref="F5:F118">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly, your Due Date needs to be greater than or equal to the Start Date." sqref="F5:F117">
       <formula1>F5&gt;=E5</formula1>
     </dataValidation>
   </dataValidations>
@@ -4188,10 +4226,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G5:G118</xm:sqref>
+          <xm:sqref>G5:G117</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="68" id="{61976558-4184-4BD1-B78A-DCBE6FDA3BC9}">
+          <x14:cfRule type="iconSet" priority="71" id="{61976558-4184-4BD1-B78A-DCBE6FDA3BC9}">
             <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4207,7 +4245,7 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>H5:H118</xm:sqref>
+          <xm:sqref>H5:H117</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>